<commit_message>
AZ and GA baselined again
</commit_message>
<xml_diff>
--- a/maps/AZ/AZ20C_candidates.xlsx
+++ b/maps/AZ/AZ20C_candidates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/dev/baseline/maps/AZ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5B30E5-E894-334B-8236-585CC8279211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A6D329-1F09-5543-836A-4F4709E0E483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="560" windowWidth="27640" windowHeight="17440" activeTab="1" xr2:uid="{D543CB8F-2BD3-B543-A7A5-5EE0E66F6344}"/>
+    <workbookView xWindow="15780" yWindow="4640" windowWidth="27640" windowHeight="17440" activeTab="1" xr2:uid="{D543CB8F-2BD3-B543-A7A5-5EE0E66F6344}"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY" sheetId="2" r:id="rId1"/>
@@ -689,7 +689,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -719,6 +719,11 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,11 +743,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="WA20C_energies" connectionId="2" xr16:uid="{23C68319-8F52-5040-8BD6-497F344644FD}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="NC20C_candidates" connectionId="1" xr16:uid="{E8ECD59F-78E1-9445-8C87-977C7625C967}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="NC20C_candidates" connectionId="1" xr16:uid="{E8ECD59F-78E1-9445-8C87-977C7625C967}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="WA20C_energies" connectionId="2" xr16:uid="{23C68319-8F52-5040-8BD6-497F344644FD}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1262,7 +1267,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1308,31 +1313,31 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2" s="29">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="25">
+      <c r="C2" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="31">
         <v>2959691.6505109998</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="32">
         <v>1.754E-2</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="32">
         <v>0</v>
       </c>
-      <c r="G2" s="21">
-        <v>1</v>
-      </c>
-      <c r="H2" s="7">
+      <c r="G2" s="32">
+        <v>1</v>
+      </c>
+      <c r="H2" s="33">
         <v>0</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="30" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1366,31 +1371,31 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="5">
         <v>98</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="23">
+      <c r="C4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="25">
         <v>2963275.4847610001</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="21">
         <v>9.4599999999999997E-3</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="21">
         <v>1.2110000000000001E-3</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="21">
         <v>0.94072699999999998</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="7">
         <v>0.303346</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="6" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>